<commit_message>
date of order added to cheque
</commit_message>
<xml_diff>
--- a/src/main/resources/cheque1.xlsx
+++ b/src/main/resources/cheque1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\virtual_D\Projects\JAVA\mezShop\back\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D66D0E57-C2E5-49F6-B708-547691066EBF}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8425A33E-1652-4C65-BE27-B54F17093A3F}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="16800" windowHeight="7250" tabRatio="0" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="35">
   <si>
     <t>Внимание! Оплата данного счета означает согласие с условиями поставки товара. Уведомление об оплате 
  обязательно, в противном случае не гарантируется наличие товара на складе. Товар отпускается по факту
@@ -57,9 +57,6 @@
     <t>Получатель</t>
   </si>
   <si>
-    <t>Счет на оплату № 2418 от 03 августа 2021 г.</t>
-  </si>
-  <si>
     <t>к  Договору №   от</t>
   </si>
   <si>
@@ -123,16 +120,13 @@
     <t>Главный (старший) бухгалтер</t>
   </si>
   <si>
-    <t>Ответственный</t>
-  </si>
-  <si>
     <t xml:space="preserve"> </t>
   </si>
   <si>
     <t xml:space="preserve">  Васильев А. Л.</t>
   </si>
   <si>
-    <t xml:space="preserve">   Подковаев Алексей</t>
+    <t>Счет на оплату от 03 августа 2021 г.</t>
   </si>
 </sst>
 </file>
@@ -533,7 +527,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="61">
+  <cellXfs count="62">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -581,6 +575,105 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="10" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="10" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="2" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -602,33 +695,12 @@
     <xf numFmtId="164" fontId="2" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -637,81 +709,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="2" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="10" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="10" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1057,8 +1054,8 @@
   </sheetPr>
   <dimension ref="A1:AM54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
-      <selection activeCell="AN26" sqref="AN26"/>
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13:AL13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.44140625" defaultRowHeight="11.4" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1069,741 +1066,741 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:38" s="1" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B1" s="17" t="s">
+      <c r="B1" s="50" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="17"/>
-      <c r="D1" s="17"/>
-      <c r="E1" s="17"/>
-      <c r="F1" s="17"/>
-      <c r="G1" s="17"/>
-      <c r="H1" s="17"/>
-      <c r="I1" s="17"/>
-      <c r="J1" s="17"/>
-      <c r="K1" s="17"/>
-      <c r="L1" s="17"/>
-      <c r="M1" s="17"/>
-      <c r="N1" s="17"/>
-      <c r="O1" s="17"/>
-      <c r="P1" s="17"/>
-      <c r="Q1" s="17"/>
-      <c r="R1" s="17"/>
-      <c r="S1" s="17"/>
-      <c r="T1" s="17"/>
-      <c r="U1" s="17"/>
-      <c r="V1" s="17"/>
-      <c r="W1" s="17"/>
-      <c r="X1" s="17"/>
-      <c r="Y1" s="17"/>
-      <c r="Z1" s="17"/>
-      <c r="AA1" s="17"/>
-      <c r="AB1" s="17"/>
-      <c r="AC1" s="17"/>
-      <c r="AD1" s="17"/>
-      <c r="AE1" s="17"/>
-      <c r="AF1" s="17"/>
-      <c r="AG1" s="17"/>
-      <c r="AH1" s="17"/>
-      <c r="AI1" s="17"/>
-      <c r="AJ1" s="17"/>
-      <c r="AK1" s="17"/>
-      <c r="AL1" s="17"/>
+      <c r="C1" s="50"/>
+      <c r="D1" s="50"/>
+      <c r="E1" s="50"/>
+      <c r="F1" s="50"/>
+      <c r="G1" s="50"/>
+      <c r="H1" s="50"/>
+      <c r="I1" s="50"/>
+      <c r="J1" s="50"/>
+      <c r="K1" s="50"/>
+      <c r="L1" s="50"/>
+      <c r="M1" s="50"/>
+      <c r="N1" s="50"/>
+      <c r="O1" s="50"/>
+      <c r="P1" s="50"/>
+      <c r="Q1" s="50"/>
+      <c r="R1" s="50"/>
+      <c r="S1" s="50"/>
+      <c r="T1" s="50"/>
+      <c r="U1" s="50"/>
+      <c r="V1" s="50"/>
+      <c r="W1" s="50"/>
+      <c r="X1" s="50"/>
+      <c r="Y1" s="50"/>
+      <c r="Z1" s="50"/>
+      <c r="AA1" s="50"/>
+      <c r="AB1" s="50"/>
+      <c r="AC1" s="50"/>
+      <c r="AD1" s="50"/>
+      <c r="AE1" s="50"/>
+      <c r="AF1" s="50"/>
+      <c r="AG1" s="50"/>
+      <c r="AH1" s="50"/>
+      <c r="AI1" s="50"/>
+      <c r="AJ1" s="50"/>
+      <c r="AK1" s="50"/>
+      <c r="AL1" s="50"/>
     </row>
     <row r="2" spans="2:38" ht="13" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="3" spans="2:38" ht="13" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B3" s="18" t="s">
+      <c r="B3" s="51" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="18"/>
-      <c r="D3" s="18"/>
-      <c r="E3" s="18"/>
-      <c r="F3" s="18"/>
-      <c r="G3" s="18"/>
-      <c r="H3" s="18"/>
-      <c r="I3" s="18"/>
-      <c r="J3" s="18"/>
-      <c r="K3" s="18"/>
-      <c r="L3" s="18"/>
-      <c r="M3" s="18"/>
-      <c r="N3" s="18"/>
-      <c r="O3" s="18"/>
-      <c r="P3" s="18"/>
-      <c r="Q3" s="18"/>
-      <c r="R3" s="18"/>
-      <c r="S3" s="18"/>
-      <c r="T3" s="22" t="s">
+      <c r="C3" s="51"/>
+      <c r="D3" s="51"/>
+      <c r="E3" s="51"/>
+      <c r="F3" s="51"/>
+      <c r="G3" s="51"/>
+      <c r="H3" s="51"/>
+      <c r="I3" s="51"/>
+      <c r="J3" s="51"/>
+      <c r="K3" s="51"/>
+      <c r="L3" s="51"/>
+      <c r="M3" s="51"/>
+      <c r="N3" s="51"/>
+      <c r="O3" s="51"/>
+      <c r="P3" s="51"/>
+      <c r="Q3" s="51"/>
+      <c r="R3" s="51"/>
+      <c r="S3" s="51"/>
+      <c r="T3" s="55" t="s">
         <v>2</v>
       </c>
-      <c r="U3" s="22"/>
-      <c r="V3" s="22"/>
-      <c r="W3" s="23">
+      <c r="U3" s="55"/>
+      <c r="V3" s="55"/>
+      <c r="W3" s="56">
         <v>44525411</v>
       </c>
-      <c r="X3" s="23"/>
-      <c r="Y3" s="23"/>
-      <c r="Z3" s="23"/>
-      <c r="AA3" s="23"/>
-      <c r="AB3" s="23"/>
-      <c r="AC3" s="23"/>
-      <c r="AD3" s="23"/>
-      <c r="AE3" s="23"/>
-      <c r="AF3" s="23"/>
-      <c r="AG3" s="23"/>
-      <c r="AH3" s="23"/>
-      <c r="AI3" s="23"/>
-      <c r="AJ3" s="23"/>
-      <c r="AK3" s="23"/>
-      <c r="AL3" s="23"/>
+      <c r="X3" s="56"/>
+      <c r="Y3" s="56"/>
+      <c r="Z3" s="56"/>
+      <c r="AA3" s="56"/>
+      <c r="AB3" s="56"/>
+      <c r="AC3" s="56"/>
+      <c r="AD3" s="56"/>
+      <c r="AE3" s="56"/>
+      <c r="AF3" s="56"/>
+      <c r="AG3" s="56"/>
+      <c r="AH3" s="56"/>
+      <c r="AI3" s="56"/>
+      <c r="AJ3" s="56"/>
+      <c r="AK3" s="56"/>
+      <c r="AL3" s="56"/>
     </row>
     <row r="4" spans="2:38" ht="11" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B4" s="19"/>
-      <c r="C4" s="20"/>
-      <c r="D4" s="20"/>
-      <c r="E4" s="20"/>
-      <c r="F4" s="20"/>
-      <c r="G4" s="20"/>
-      <c r="H4" s="20"/>
-      <c r="I4" s="20"/>
-      <c r="J4" s="20"/>
-      <c r="K4" s="20"/>
-      <c r="L4" s="20"/>
-      <c r="M4" s="20"/>
-      <c r="N4" s="20"/>
-      <c r="O4" s="20"/>
-      <c r="P4" s="20"/>
-      <c r="Q4" s="20"/>
-      <c r="R4" s="20"/>
-      <c r="S4" s="21"/>
-      <c r="T4" s="24" t="s">
+      <c r="B4" s="52"/>
+      <c r="C4" s="53"/>
+      <c r="D4" s="53"/>
+      <c r="E4" s="53"/>
+      <c r="F4" s="53"/>
+      <c r="G4" s="53"/>
+      <c r="H4" s="53"/>
+      <c r="I4" s="53"/>
+      <c r="J4" s="53"/>
+      <c r="K4" s="53"/>
+      <c r="L4" s="53"/>
+      <c r="M4" s="53"/>
+      <c r="N4" s="53"/>
+      <c r="O4" s="53"/>
+      <c r="P4" s="53"/>
+      <c r="Q4" s="53"/>
+      <c r="R4" s="53"/>
+      <c r="S4" s="54"/>
+      <c r="T4" s="42" t="s">
         <v>3</v>
       </c>
-      <c r="U4" s="24"/>
-      <c r="V4" s="24"/>
-      <c r="W4" s="28" t="s">
+      <c r="U4" s="42"/>
+      <c r="V4" s="42"/>
+      <c r="W4" s="57" t="s">
         <v>4</v>
       </c>
-      <c r="X4" s="28"/>
-      <c r="Y4" s="28"/>
-      <c r="Z4" s="28"/>
-      <c r="AA4" s="28"/>
-      <c r="AB4" s="28"/>
-      <c r="AC4" s="28"/>
-      <c r="AD4" s="28"/>
-      <c r="AE4" s="28"/>
-      <c r="AF4" s="28"/>
-      <c r="AG4" s="28"/>
-      <c r="AH4" s="28"/>
-      <c r="AI4" s="28"/>
-      <c r="AJ4" s="28"/>
-      <c r="AK4" s="28"/>
-      <c r="AL4" s="28"/>
+      <c r="X4" s="57"/>
+      <c r="Y4" s="57"/>
+      <c r="Z4" s="57"/>
+      <c r="AA4" s="57"/>
+      <c r="AB4" s="57"/>
+      <c r="AC4" s="57"/>
+      <c r="AD4" s="57"/>
+      <c r="AE4" s="57"/>
+      <c r="AF4" s="57"/>
+      <c r="AG4" s="57"/>
+      <c r="AH4" s="57"/>
+      <c r="AI4" s="57"/>
+      <c r="AJ4" s="57"/>
+      <c r="AK4" s="57"/>
+      <c r="AL4" s="57"/>
     </row>
     <row r="5" spans="2:38" ht="11" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B5" s="29" t="s">
+      <c r="B5" s="58" t="s">
         <v>5</v>
       </c>
-      <c r="C5" s="29"/>
-      <c r="D5" s="29"/>
-      <c r="E5" s="29"/>
-      <c r="F5" s="29"/>
-      <c r="G5" s="29"/>
-      <c r="H5" s="29"/>
-      <c r="I5" s="29"/>
-      <c r="J5" s="29"/>
-      <c r="K5" s="29"/>
-      <c r="L5" s="29"/>
-      <c r="M5" s="29"/>
-      <c r="N5" s="29"/>
-      <c r="O5" s="29"/>
-      <c r="P5" s="29"/>
-      <c r="Q5" s="29"/>
-      <c r="R5" s="29"/>
-      <c r="S5" s="29"/>
-      <c r="T5" s="25"/>
-      <c r="U5" s="26"/>
-      <c r="V5" s="27"/>
-      <c r="W5" s="25"/>
-      <c r="X5" s="26"/>
-      <c r="Y5" s="26"/>
-      <c r="Z5" s="26"/>
-      <c r="AA5" s="26"/>
-      <c r="AB5" s="26"/>
-      <c r="AC5" s="26"/>
-      <c r="AD5" s="26"/>
-      <c r="AE5" s="26"/>
-      <c r="AF5" s="26"/>
-      <c r="AG5" s="26"/>
-      <c r="AH5" s="26"/>
-      <c r="AI5" s="26"/>
-      <c r="AJ5" s="26"/>
-      <c r="AK5" s="26"/>
-      <c r="AL5" s="27"/>
+      <c r="C5" s="58"/>
+      <c r="D5" s="58"/>
+      <c r="E5" s="58"/>
+      <c r="F5" s="58"/>
+      <c r="G5" s="58"/>
+      <c r="H5" s="58"/>
+      <c r="I5" s="58"/>
+      <c r="J5" s="58"/>
+      <c r="K5" s="58"/>
+      <c r="L5" s="58"/>
+      <c r="M5" s="58"/>
+      <c r="N5" s="58"/>
+      <c r="O5" s="58"/>
+      <c r="P5" s="58"/>
+      <c r="Q5" s="58"/>
+      <c r="R5" s="58"/>
+      <c r="S5" s="58"/>
+      <c r="T5" s="46"/>
+      <c r="U5" s="47"/>
+      <c r="V5" s="48"/>
+      <c r="W5" s="46"/>
+      <c r="X5" s="47"/>
+      <c r="Y5" s="47"/>
+      <c r="Z5" s="47"/>
+      <c r="AA5" s="47"/>
+      <c r="AB5" s="47"/>
+      <c r="AC5" s="47"/>
+      <c r="AD5" s="47"/>
+      <c r="AE5" s="47"/>
+      <c r="AF5" s="47"/>
+      <c r="AG5" s="47"/>
+      <c r="AH5" s="47"/>
+      <c r="AI5" s="47"/>
+      <c r="AJ5" s="47"/>
+      <c r="AK5" s="47"/>
+      <c r="AL5" s="48"/>
     </row>
     <row r="6" spans="2:38" ht="13" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B6" s="35" t="s">
+      <c r="B6" s="61" t="s">
         <v>6</v>
       </c>
-      <c r="C6" s="35"/>
-      <c r="D6" s="36">
+      <c r="C6" s="61"/>
+      <c r="D6" s="41">
         <v>7701590872</v>
       </c>
-      <c r="E6" s="36"/>
-      <c r="F6" s="36"/>
-      <c r="G6" s="36"/>
-      <c r="H6" s="36"/>
-      <c r="I6" s="36"/>
-      <c r="J6" s="36"/>
-      <c r="K6" s="35" t="s">
+      <c r="E6" s="41"/>
+      <c r="F6" s="41"/>
+      <c r="G6" s="41"/>
+      <c r="H6" s="41"/>
+      <c r="I6" s="41"/>
+      <c r="J6" s="41"/>
+      <c r="K6" s="61" t="s">
         <v>7</v>
       </c>
-      <c r="L6" s="35"/>
-      <c r="M6" s="36">
+      <c r="L6" s="61"/>
+      <c r="M6" s="41">
         <v>773601001</v>
       </c>
-      <c r="N6" s="36"/>
-      <c r="O6" s="36"/>
-      <c r="P6" s="36"/>
-      <c r="Q6" s="36"/>
-      <c r="R6" s="36"/>
-      <c r="S6" s="36"/>
-      <c r="T6" s="24" t="s">
+      <c r="N6" s="41"/>
+      <c r="O6" s="41"/>
+      <c r="P6" s="41"/>
+      <c r="Q6" s="41"/>
+      <c r="R6" s="41"/>
+      <c r="S6" s="41"/>
+      <c r="T6" s="42" t="s">
         <v>3</v>
       </c>
-      <c r="U6" s="24"/>
-      <c r="V6" s="24"/>
-      <c r="W6" s="24" t="s">
+      <c r="U6" s="42"/>
+      <c r="V6" s="42"/>
+      <c r="W6" s="42" t="s">
         <v>8</v>
       </c>
-      <c r="X6" s="24"/>
-      <c r="Y6" s="24"/>
-      <c r="Z6" s="24"/>
-      <c r="AA6" s="24"/>
-      <c r="AB6" s="24"/>
-      <c r="AC6" s="24"/>
-      <c r="AD6" s="24"/>
-      <c r="AE6" s="24"/>
-      <c r="AF6" s="24"/>
-      <c r="AG6" s="24"/>
-      <c r="AH6" s="24"/>
-      <c r="AI6" s="24"/>
-      <c r="AJ6" s="24"/>
-      <c r="AK6" s="24"/>
-      <c r="AL6" s="24"/>
+      <c r="X6" s="42"/>
+      <c r="Y6" s="42"/>
+      <c r="Z6" s="42"/>
+      <c r="AA6" s="42"/>
+      <c r="AB6" s="42"/>
+      <c r="AC6" s="42"/>
+      <c r="AD6" s="42"/>
+      <c r="AE6" s="42"/>
+      <c r="AF6" s="42"/>
+      <c r="AG6" s="42"/>
+      <c r="AH6" s="42"/>
+      <c r="AI6" s="42"/>
+      <c r="AJ6" s="42"/>
+      <c r="AK6" s="42"/>
+      <c r="AL6" s="42"/>
     </row>
     <row r="7" spans="2:38" ht="13" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B7" s="18" t="s">
+      <c r="B7" s="51" t="s">
         <v>9</v>
       </c>
-      <c r="C7" s="18"/>
-      <c r="D7" s="18"/>
-      <c r="E7" s="18"/>
-      <c r="F7" s="18"/>
-      <c r="G7" s="18"/>
-      <c r="H7" s="18"/>
-      <c r="I7" s="18"/>
-      <c r="J7" s="18"/>
-      <c r="K7" s="18"/>
-      <c r="L7" s="18"/>
-      <c r="M7" s="18"/>
-      <c r="N7" s="18"/>
-      <c r="O7" s="18"/>
-      <c r="P7" s="18"/>
-      <c r="Q7" s="18"/>
-      <c r="R7" s="18"/>
-      <c r="S7" s="18"/>
-      <c r="T7" s="30"/>
-      <c r="U7" s="31"/>
-      <c r="V7" s="32"/>
-      <c r="W7" s="30"/>
-      <c r="X7" s="31"/>
-      <c r="Y7" s="31"/>
-      <c r="Z7" s="31"/>
-      <c r="AA7" s="31"/>
-      <c r="AB7" s="31"/>
-      <c r="AC7" s="31"/>
-      <c r="AD7" s="31"/>
-      <c r="AE7" s="31"/>
-      <c r="AF7" s="31"/>
-      <c r="AG7" s="31"/>
-      <c r="AH7" s="31"/>
-      <c r="AI7" s="31"/>
-      <c r="AJ7" s="31"/>
-      <c r="AK7" s="31"/>
-      <c r="AL7" s="32"/>
+      <c r="C7" s="51"/>
+      <c r="D7" s="51"/>
+      <c r="E7" s="51"/>
+      <c r="F7" s="51"/>
+      <c r="G7" s="51"/>
+      <c r="H7" s="51"/>
+      <c r="I7" s="51"/>
+      <c r="J7" s="51"/>
+      <c r="K7" s="51"/>
+      <c r="L7" s="51"/>
+      <c r="M7" s="51"/>
+      <c r="N7" s="51"/>
+      <c r="O7" s="51"/>
+      <c r="P7" s="51"/>
+      <c r="Q7" s="51"/>
+      <c r="R7" s="51"/>
+      <c r="S7" s="51"/>
+      <c r="T7" s="43"/>
+      <c r="U7" s="44"/>
+      <c r="V7" s="45"/>
+      <c r="W7" s="43"/>
+      <c r="X7" s="44"/>
+      <c r="Y7" s="44"/>
+      <c r="Z7" s="44"/>
+      <c r="AA7" s="44"/>
+      <c r="AB7" s="44"/>
+      <c r="AC7" s="44"/>
+      <c r="AD7" s="44"/>
+      <c r="AE7" s="44"/>
+      <c r="AF7" s="44"/>
+      <c r="AG7" s="44"/>
+      <c r="AH7" s="44"/>
+      <c r="AI7" s="44"/>
+      <c r="AJ7" s="44"/>
+      <c r="AK7" s="44"/>
+      <c r="AL7" s="45"/>
     </row>
     <row r="8" spans="2:38" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B8" s="19"/>
-      <c r="C8" s="20"/>
-      <c r="D8" s="20"/>
-      <c r="E8" s="20"/>
-      <c r="F8" s="20"/>
-      <c r="G8" s="20"/>
-      <c r="H8" s="20"/>
-      <c r="I8" s="20"/>
-      <c r="J8" s="20"/>
-      <c r="K8" s="20"/>
-      <c r="L8" s="20"/>
-      <c r="M8" s="20"/>
-      <c r="N8" s="20"/>
-      <c r="O8" s="20"/>
-      <c r="P8" s="20"/>
-      <c r="Q8" s="20"/>
-      <c r="R8" s="20"/>
-      <c r="S8" s="21"/>
-      <c r="T8" s="30"/>
-      <c r="U8" s="31"/>
-      <c r="V8" s="32"/>
-      <c r="W8" s="30"/>
-      <c r="X8" s="31"/>
-      <c r="Y8" s="31"/>
-      <c r="Z8" s="31"/>
-      <c r="AA8" s="31"/>
-      <c r="AB8" s="31"/>
-      <c r="AC8" s="31"/>
-      <c r="AD8" s="31"/>
-      <c r="AE8" s="31"/>
-      <c r="AF8" s="31"/>
-      <c r="AG8" s="31"/>
-      <c r="AH8" s="31"/>
-      <c r="AI8" s="31"/>
-      <c r="AJ8" s="31"/>
-      <c r="AK8" s="31"/>
-      <c r="AL8" s="32"/>
+      <c r="B8" s="52"/>
+      <c r="C8" s="53"/>
+      <c r="D8" s="53"/>
+      <c r="E8" s="53"/>
+      <c r="F8" s="53"/>
+      <c r="G8" s="53"/>
+      <c r="H8" s="53"/>
+      <c r="I8" s="53"/>
+      <c r="J8" s="53"/>
+      <c r="K8" s="53"/>
+      <c r="L8" s="53"/>
+      <c r="M8" s="53"/>
+      <c r="N8" s="53"/>
+      <c r="O8" s="53"/>
+      <c r="P8" s="53"/>
+      <c r="Q8" s="53"/>
+      <c r="R8" s="53"/>
+      <c r="S8" s="54"/>
+      <c r="T8" s="43"/>
+      <c r="U8" s="44"/>
+      <c r="V8" s="45"/>
+      <c r="W8" s="43"/>
+      <c r="X8" s="44"/>
+      <c r="Y8" s="44"/>
+      <c r="Z8" s="44"/>
+      <c r="AA8" s="44"/>
+      <c r="AB8" s="44"/>
+      <c r="AC8" s="44"/>
+      <c r="AD8" s="44"/>
+      <c r="AE8" s="44"/>
+      <c r="AF8" s="44"/>
+      <c r="AG8" s="44"/>
+      <c r="AH8" s="44"/>
+      <c r="AI8" s="44"/>
+      <c r="AJ8" s="44"/>
+      <c r="AK8" s="44"/>
+      <c r="AL8" s="45"/>
     </row>
     <row r="9" spans="2:38" ht="11" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B9" s="29" t="s">
+      <c r="B9" s="58" t="s">
         <v>10</v>
       </c>
-      <c r="C9" s="29"/>
-      <c r="D9" s="29"/>
-      <c r="E9" s="29"/>
-      <c r="F9" s="29"/>
-      <c r="G9" s="29"/>
-      <c r="H9" s="29"/>
-      <c r="I9" s="29"/>
-      <c r="J9" s="29"/>
-      <c r="K9" s="29"/>
-      <c r="L9" s="29"/>
-      <c r="M9" s="29"/>
-      <c r="N9" s="29"/>
-      <c r="O9" s="29"/>
-      <c r="P9" s="29"/>
-      <c r="Q9" s="29"/>
-      <c r="R9" s="29"/>
-      <c r="S9" s="29"/>
-      <c r="T9" s="25"/>
-      <c r="U9" s="26"/>
-      <c r="V9" s="27"/>
-      <c r="W9" s="25"/>
-      <c r="X9" s="26"/>
-      <c r="Y9" s="26"/>
-      <c r="Z9" s="26"/>
-      <c r="AA9" s="26"/>
-      <c r="AB9" s="26"/>
-      <c r="AC9" s="26"/>
-      <c r="AD9" s="26"/>
-      <c r="AE9" s="26"/>
-      <c r="AF9" s="26"/>
-      <c r="AG9" s="26"/>
-      <c r="AH9" s="26"/>
-      <c r="AI9" s="26"/>
-      <c r="AJ9" s="26"/>
-      <c r="AK9" s="26"/>
-      <c r="AL9" s="27"/>
+      <c r="C9" s="58"/>
+      <c r="D9" s="58"/>
+      <c r="E9" s="58"/>
+      <c r="F9" s="58"/>
+      <c r="G9" s="58"/>
+      <c r="H9" s="58"/>
+      <c r="I9" s="58"/>
+      <c r="J9" s="58"/>
+      <c r="K9" s="58"/>
+      <c r="L9" s="58"/>
+      <c r="M9" s="58"/>
+      <c r="N9" s="58"/>
+      <c r="O9" s="58"/>
+      <c r="P9" s="58"/>
+      <c r="Q9" s="58"/>
+      <c r="R9" s="58"/>
+      <c r="S9" s="58"/>
+      <c r="T9" s="46"/>
+      <c r="U9" s="47"/>
+      <c r="V9" s="48"/>
+      <c r="W9" s="46"/>
+      <c r="X9" s="47"/>
+      <c r="Y9" s="47"/>
+      <c r="Z9" s="47"/>
+      <c r="AA9" s="47"/>
+      <c r="AB9" s="47"/>
+      <c r="AC9" s="47"/>
+      <c r="AD9" s="47"/>
+      <c r="AE9" s="47"/>
+      <c r="AF9" s="47"/>
+      <c r="AG9" s="47"/>
+      <c r="AH9" s="47"/>
+      <c r="AI9" s="47"/>
+      <c r="AJ9" s="47"/>
+      <c r="AK9" s="47"/>
+      <c r="AL9" s="48"/>
     </row>
     <row r="11" spans="2:38" s="1" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B11" s="33" t="s">
-        <v>11</v>
-      </c>
-      <c r="C11" s="33"/>
-      <c r="D11" s="33"/>
-      <c r="E11" s="33"/>
-      <c r="F11" s="33"/>
-      <c r="G11" s="33"/>
-      <c r="H11" s="33"/>
-      <c r="I11" s="33"/>
-      <c r="J11" s="33"/>
-      <c r="K11" s="33"/>
-      <c r="L11" s="33"/>
-      <c r="M11" s="33"/>
-      <c r="N11" s="33"/>
-      <c r="O11" s="33"/>
-      <c r="P11" s="33"/>
-      <c r="Q11" s="33"/>
-      <c r="R11" s="33"/>
-      <c r="S11" s="33"/>
-      <c r="T11" s="33"/>
-      <c r="U11" s="33"/>
-      <c r="V11" s="33"/>
-      <c r="W11" s="33"/>
-      <c r="X11" s="33"/>
-      <c r="Y11" s="33"/>
-      <c r="Z11" s="33"/>
-      <c r="AA11" s="33"/>
-      <c r="AB11" s="33"/>
-      <c r="AC11" s="33"/>
-      <c r="AD11" s="33"/>
-      <c r="AE11" s="33"/>
-      <c r="AF11" s="33"/>
-      <c r="AG11" s="33"/>
-      <c r="AH11" s="33"/>
-      <c r="AI11" s="33"/>
-      <c r="AJ11" s="33"/>
-      <c r="AK11" s="33"/>
-      <c r="AL11" s="33"/>
+      <c r="B11" s="59" t="s">
+        <v>34</v>
+      </c>
+      <c r="C11" s="59"/>
+      <c r="D11" s="59"/>
+      <c r="E11" s="59"/>
+      <c r="F11" s="59"/>
+      <c r="G11" s="59"/>
+      <c r="H11" s="59"/>
+      <c r="I11" s="59"/>
+      <c r="J11" s="59"/>
+      <c r="K11" s="59"/>
+      <c r="L11" s="59"/>
+      <c r="M11" s="59"/>
+      <c r="N11" s="59"/>
+      <c r="O11" s="59"/>
+      <c r="P11" s="59"/>
+      <c r="Q11" s="59"/>
+      <c r="R11" s="59"/>
+      <c r="S11" s="59"/>
+      <c r="T11" s="59"/>
+      <c r="U11" s="59"/>
+      <c r="V11" s="59"/>
+      <c r="W11" s="59"/>
+      <c r="X11" s="59"/>
+      <c r="Y11" s="59"/>
+      <c r="Z11" s="59"/>
+      <c r="AA11" s="59"/>
+      <c r="AB11" s="59"/>
+      <c r="AC11" s="59"/>
+      <c r="AD11" s="59"/>
+      <c r="AE11" s="59"/>
+      <c r="AF11" s="59"/>
+      <c r="AG11" s="59"/>
+      <c r="AH11" s="59"/>
+      <c r="AI11" s="59"/>
+      <c r="AJ11" s="59"/>
+      <c r="AK11" s="59"/>
+      <c r="AL11" s="59"/>
     </row>
     <row r="12" spans="2:38" s="1" customFormat="1" ht="9" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="13" spans="2:38" ht="16" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B13" s="34" t="s">
-        <v>12</v>
-      </c>
-      <c r="C13" s="34"/>
-      <c r="D13" s="34"/>
-      <c r="E13" s="34"/>
-      <c r="F13" s="34"/>
-      <c r="G13" s="34"/>
-      <c r="H13" s="34"/>
-      <c r="I13" s="34"/>
-      <c r="J13" s="34"/>
-      <c r="K13" s="34"/>
-      <c r="L13" s="34"/>
-      <c r="M13" s="34"/>
-      <c r="N13" s="34"/>
-      <c r="O13" s="34"/>
-      <c r="P13" s="34"/>
-      <c r="Q13" s="34"/>
-      <c r="R13" s="34"/>
-      <c r="S13" s="34"/>
-      <c r="T13" s="34"/>
-      <c r="U13" s="34"/>
-      <c r="V13" s="34"/>
-      <c r="W13" s="34"/>
-      <c r="X13" s="34"/>
-      <c r="Y13" s="34"/>
-      <c r="Z13" s="34"/>
-      <c r="AA13" s="34"/>
-      <c r="AB13" s="34"/>
-      <c r="AC13" s="34"/>
-      <c r="AD13" s="34"/>
-      <c r="AE13" s="34"/>
-      <c r="AF13" s="34"/>
-      <c r="AG13" s="34"/>
-      <c r="AH13" s="34"/>
-      <c r="AI13" s="34"/>
-      <c r="AJ13" s="34"/>
-      <c r="AK13" s="34"/>
-      <c r="AL13" s="34"/>
+      <c r="B13" s="60" t="s">
+        <v>11</v>
+      </c>
+      <c r="C13" s="60"/>
+      <c r="D13" s="60"/>
+      <c r="E13" s="60"/>
+      <c r="F13" s="60"/>
+      <c r="G13" s="60"/>
+      <c r="H13" s="60"/>
+      <c r="I13" s="60"/>
+      <c r="J13" s="60"/>
+      <c r="K13" s="60"/>
+      <c r="L13" s="60"/>
+      <c r="M13" s="60"/>
+      <c r="N13" s="60"/>
+      <c r="O13" s="60"/>
+      <c r="P13" s="60"/>
+      <c r="Q13" s="60"/>
+      <c r="R13" s="60"/>
+      <c r="S13" s="60"/>
+      <c r="T13" s="60"/>
+      <c r="U13" s="60"/>
+      <c r="V13" s="60"/>
+      <c r="W13" s="60"/>
+      <c r="X13" s="60"/>
+      <c r="Y13" s="60"/>
+      <c r="Z13" s="60"/>
+      <c r="AA13" s="60"/>
+      <c r="AB13" s="60"/>
+      <c r="AC13" s="60"/>
+      <c r="AD13" s="60"/>
+      <c r="AE13" s="60"/>
+      <c r="AF13" s="60"/>
+      <c r="AG13" s="60"/>
+      <c r="AH13" s="60"/>
+      <c r="AI13" s="60"/>
+      <c r="AJ13" s="60"/>
+      <c r="AK13" s="60"/>
+      <c r="AL13" s="60"/>
     </row>
     <row r="14" spans="2:38" s="1" customFormat="1" ht="10" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="15" spans="2:38" s="1" customFormat="1" ht="37" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B15" s="37" t="s">
-        <v>13</v>
-      </c>
-      <c r="C15" s="37"/>
-      <c r="D15" s="37"/>
-      <c r="E15" s="37"/>
-      <c r="F15" s="37"/>
-      <c r="G15" s="37"/>
-      <c r="H15" s="37"/>
-      <c r="I15" s="37"/>
-      <c r="J15" s="37"/>
-      <c r="K15" s="37"/>
-      <c r="L15" s="37"/>
-      <c r="M15" s="37"/>
-      <c r="N15" s="37"/>
-      <c r="O15" s="37"/>
-      <c r="P15" s="37"/>
-      <c r="Q15" s="37"/>
-      <c r="R15" s="37"/>
-      <c r="S15" s="37"/>
-      <c r="T15" s="37"/>
-      <c r="U15" s="37"/>
-      <c r="V15" s="37"/>
-      <c r="W15" s="37"/>
-      <c r="X15" s="37"/>
-      <c r="Y15" s="37"/>
-      <c r="Z15" s="37"/>
-      <c r="AA15" s="37"/>
-      <c r="AB15" s="37"/>
-      <c r="AC15" s="37"/>
-      <c r="AD15" s="37"/>
-      <c r="AE15" s="37"/>
-      <c r="AF15" s="37"/>
-      <c r="AG15" s="37"/>
-      <c r="AH15" s="37"/>
-      <c r="AI15" s="37"/>
-      <c r="AJ15" s="37"/>
-      <c r="AK15" s="37"/>
-      <c r="AL15" s="37"/>
+      <c r="B15" s="49" t="s">
+        <v>12</v>
+      </c>
+      <c r="C15" s="49"/>
+      <c r="D15" s="49"/>
+      <c r="E15" s="49"/>
+      <c r="F15" s="49"/>
+      <c r="G15" s="49"/>
+      <c r="H15" s="49"/>
+      <c r="I15" s="49"/>
+      <c r="J15" s="49"/>
+      <c r="K15" s="49"/>
+      <c r="L15" s="49"/>
+      <c r="M15" s="49"/>
+      <c r="N15" s="49"/>
+      <c r="O15" s="49"/>
+      <c r="P15" s="49"/>
+      <c r="Q15" s="49"/>
+      <c r="R15" s="49"/>
+      <c r="S15" s="49"/>
+      <c r="T15" s="49"/>
+      <c r="U15" s="49"/>
+      <c r="V15" s="49"/>
+      <c r="W15" s="49"/>
+      <c r="X15" s="49"/>
+      <c r="Y15" s="49"/>
+      <c r="Z15" s="49"/>
+      <c r="AA15" s="49"/>
+      <c r="AB15" s="49"/>
+      <c r="AC15" s="49"/>
+      <c r="AD15" s="49"/>
+      <c r="AE15" s="49"/>
+      <c r="AF15" s="49"/>
+      <c r="AG15" s="49"/>
+      <c r="AH15" s="49"/>
+      <c r="AI15" s="49"/>
+      <c r="AJ15" s="49"/>
+      <c r="AK15" s="49"/>
+      <c r="AL15" s="49"/>
     </row>
     <row r="16" spans="2:38" s="1" customFormat="1" ht="7" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="17" spans="2:38" ht="38" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B17" s="38" t="s">
+      <c r="B17" s="32" t="s">
+        <v>13</v>
+      </c>
+      <c r="C17" s="32"/>
+      <c r="D17" s="32"/>
+      <c r="E17" s="32"/>
+      <c r="F17" s="32"/>
+      <c r="G17" s="32"/>
+      <c r="H17" s="33" t="s">
         <v>14</v>
       </c>
-      <c r="C17" s="38"/>
-      <c r="D17" s="38"/>
-      <c r="E17" s="38"/>
-      <c r="F17" s="38"/>
-      <c r="G17" s="38"/>
-      <c r="H17" s="39" t="s">
-        <v>15</v>
-      </c>
-      <c r="I17" s="39"/>
-      <c r="J17" s="39"/>
-      <c r="K17" s="39"/>
-      <c r="L17" s="39"/>
-      <c r="M17" s="39"/>
-      <c r="N17" s="39"/>
-      <c r="O17" s="39"/>
-      <c r="P17" s="39"/>
-      <c r="Q17" s="39"/>
-      <c r="R17" s="39"/>
-      <c r="S17" s="39"/>
-      <c r="T17" s="39"/>
-      <c r="U17" s="39"/>
-      <c r="V17" s="39"/>
-      <c r="W17" s="39"/>
-      <c r="X17" s="39"/>
-      <c r="Y17" s="39"/>
-      <c r="Z17" s="39"/>
-      <c r="AA17" s="39"/>
-      <c r="AB17" s="39"/>
-      <c r="AC17" s="39"/>
-      <c r="AD17" s="39"/>
-      <c r="AE17" s="39"/>
-      <c r="AF17" s="39"/>
-      <c r="AG17" s="39"/>
-      <c r="AH17" s="39"/>
-      <c r="AI17" s="39"/>
-      <c r="AJ17" s="39"/>
-      <c r="AK17" s="39"/>
-      <c r="AL17" s="39"/>
+      <c r="I17" s="33"/>
+      <c r="J17" s="33"/>
+      <c r="K17" s="33"/>
+      <c r="L17" s="33"/>
+      <c r="M17" s="33"/>
+      <c r="N17" s="33"/>
+      <c r="O17" s="33"/>
+      <c r="P17" s="33"/>
+      <c r="Q17" s="33"/>
+      <c r="R17" s="33"/>
+      <c r="S17" s="33"/>
+      <c r="T17" s="33"/>
+      <c r="U17" s="33"/>
+      <c r="V17" s="33"/>
+      <c r="W17" s="33"/>
+      <c r="X17" s="33"/>
+      <c r="Y17" s="33"/>
+      <c r="Z17" s="33"/>
+      <c r="AA17" s="33"/>
+      <c r="AB17" s="33"/>
+      <c r="AC17" s="33"/>
+      <c r="AD17" s="33"/>
+      <c r="AE17" s="33"/>
+      <c r="AF17" s="33"/>
+      <c r="AG17" s="33"/>
+      <c r="AH17" s="33"/>
+      <c r="AI17" s="33"/>
+      <c r="AJ17" s="33"/>
+      <c r="AK17" s="33"/>
+      <c r="AL17" s="33"/>
     </row>
     <row r="18" spans="2:38" ht="13" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="19" spans="2:38" ht="38" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B19" s="38" t="s">
+      <c r="B19" s="32" t="s">
+        <v>15</v>
+      </c>
+      <c r="C19" s="32"/>
+      <c r="D19" s="32"/>
+      <c r="E19" s="32"/>
+      <c r="F19" s="32"/>
+      <c r="G19" s="32"/>
+      <c r="H19" s="33" t="s">
+        <v>14</v>
+      </c>
+      <c r="I19" s="33"/>
+      <c r="J19" s="33"/>
+      <c r="K19" s="33"/>
+      <c r="L19" s="33"/>
+      <c r="M19" s="33"/>
+      <c r="N19" s="33"/>
+      <c r="O19" s="33"/>
+      <c r="P19" s="33"/>
+      <c r="Q19" s="33"/>
+      <c r="R19" s="33"/>
+      <c r="S19" s="33"/>
+      <c r="T19" s="33"/>
+      <c r="U19" s="33"/>
+      <c r="V19" s="33"/>
+      <c r="W19" s="33"/>
+      <c r="X19" s="33"/>
+      <c r="Y19" s="33"/>
+      <c r="Z19" s="33"/>
+      <c r="AA19" s="33"/>
+      <c r="AB19" s="33"/>
+      <c r="AC19" s="33"/>
+      <c r="AD19" s="33"/>
+      <c r="AE19" s="33"/>
+      <c r="AF19" s="33"/>
+      <c r="AG19" s="33"/>
+      <c r="AH19" s="33"/>
+      <c r="AI19" s="33"/>
+      <c r="AJ19" s="33"/>
+      <c r="AK19" s="33"/>
+      <c r="AL19" s="33"/>
+    </row>
+    <row r="21" spans="2:38" ht="22" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B21" s="32" t="s">
         <v>16</v>
       </c>
-      <c r="C19" s="38"/>
-      <c r="D19" s="38"/>
-      <c r="E19" s="38"/>
-      <c r="F19" s="38"/>
-      <c r="G19" s="38"/>
-      <c r="H19" s="39" t="s">
-        <v>15</v>
-      </c>
-      <c r="I19" s="39"/>
-      <c r="J19" s="39"/>
-      <c r="K19" s="39"/>
-      <c r="L19" s="39"/>
-      <c r="M19" s="39"/>
-      <c r="N19" s="39"/>
-      <c r="O19" s="39"/>
-      <c r="P19" s="39"/>
-      <c r="Q19" s="39"/>
-      <c r="R19" s="39"/>
-      <c r="S19" s="39"/>
-      <c r="T19" s="39"/>
-      <c r="U19" s="39"/>
-      <c r="V19" s="39"/>
-      <c r="W19" s="39"/>
-      <c r="X19" s="39"/>
-      <c r="Y19" s="39"/>
-      <c r="Z19" s="39"/>
-      <c r="AA19" s="39"/>
-      <c r="AB19" s="39"/>
-      <c r="AC19" s="39"/>
-      <c r="AD19" s="39"/>
-      <c r="AE19" s="39"/>
-      <c r="AF19" s="39"/>
-      <c r="AG19" s="39"/>
-      <c r="AH19" s="39"/>
-      <c r="AI19" s="39"/>
-      <c r="AJ19" s="39"/>
-      <c r="AK19" s="39"/>
-      <c r="AL19" s="39"/>
-    </row>
-    <row r="21" spans="2:38" ht="22" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B21" s="38" t="s">
-        <v>17</v>
-      </c>
-      <c r="C21" s="38"/>
-      <c r="D21" s="38"/>
-      <c r="E21" s="38"/>
-      <c r="F21" s="38"/>
-      <c r="G21" s="38"/>
-      <c r="H21" s="39"/>
-      <c r="I21" s="39"/>
-      <c r="J21" s="39"/>
-      <c r="K21" s="39"/>
-      <c r="L21" s="39"/>
-      <c r="M21" s="39"/>
-      <c r="N21" s="39"/>
-      <c r="O21" s="39"/>
-      <c r="P21" s="39"/>
-      <c r="Q21" s="39"/>
-      <c r="R21" s="39"/>
-      <c r="S21" s="39"/>
-      <c r="T21" s="39"/>
-      <c r="U21" s="39"/>
-      <c r="V21" s="39"/>
-      <c r="W21" s="39"/>
-      <c r="X21" s="39"/>
-      <c r="Y21" s="39"/>
-      <c r="Z21" s="39"/>
-      <c r="AA21" s="39"/>
-      <c r="AB21" s="39"/>
-      <c r="AC21" s="39"/>
-      <c r="AD21" s="39"/>
-      <c r="AE21" s="39"/>
-      <c r="AF21" s="39"/>
-      <c r="AG21" s="39"/>
-      <c r="AH21" s="39"/>
-      <c r="AI21" s="39"/>
-      <c r="AJ21" s="39"/>
-      <c r="AK21" s="39"/>
-      <c r="AL21" s="39"/>
+      <c r="C21" s="32"/>
+      <c r="D21" s="32"/>
+      <c r="E21" s="32"/>
+      <c r="F21" s="32"/>
+      <c r="G21" s="32"/>
+      <c r="H21" s="33"/>
+      <c r="I21" s="33"/>
+      <c r="J21" s="33"/>
+      <c r="K21" s="33"/>
+      <c r="L21" s="33"/>
+      <c r="M21" s="33"/>
+      <c r="N21" s="33"/>
+      <c r="O21" s="33"/>
+      <c r="P21" s="33"/>
+      <c r="Q21" s="33"/>
+      <c r="R21" s="33"/>
+      <c r="S21" s="33"/>
+      <c r="T21" s="33"/>
+      <c r="U21" s="33"/>
+      <c r="V21" s="33"/>
+      <c r="W21" s="33"/>
+      <c r="X21" s="33"/>
+      <c r="Y21" s="33"/>
+      <c r="Z21" s="33"/>
+      <c r="AA21" s="33"/>
+      <c r="AB21" s="33"/>
+      <c r="AC21" s="33"/>
+      <c r="AD21" s="33"/>
+      <c r="AE21" s="33"/>
+      <c r="AF21" s="33"/>
+      <c r="AG21" s="33"/>
+      <c r="AH21" s="33"/>
+      <c r="AI21" s="33"/>
+      <c r="AJ21" s="33"/>
+      <c r="AK21" s="33"/>
+      <c r="AL21" s="33"/>
     </row>
     <row r="22" spans="2:38" ht="13" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="23" spans="2:38" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B23" s="38" t="s">
-        <v>18</v>
-      </c>
-      <c r="C23" s="38"/>
-      <c r="D23" s="38"/>
-      <c r="E23" s="38"/>
-      <c r="F23" s="38"/>
-      <c r="G23" s="38"/>
-      <c r="H23" s="43"/>
-      <c r="I23" s="43"/>
-      <c r="J23" s="43"/>
-      <c r="K23" s="43"/>
-      <c r="L23" s="43"/>
-      <c r="M23" s="43"/>
-      <c r="N23" s="43"/>
-      <c r="O23" s="43"/>
-      <c r="P23" s="43"/>
-      <c r="Q23" s="43"/>
-      <c r="R23" s="43"/>
-      <c r="S23" s="43"/>
-      <c r="T23" s="43"/>
-      <c r="U23" s="43"/>
-      <c r="V23" s="43"/>
-      <c r="W23" s="43"/>
-      <c r="X23" s="43"/>
-      <c r="Y23" s="43"/>
-      <c r="Z23" s="43"/>
-      <c r="AA23" s="43"/>
-      <c r="AB23" s="43"/>
-      <c r="AC23" s="43"/>
-      <c r="AD23" s="43"/>
-      <c r="AE23" s="43"/>
-      <c r="AF23" s="43"/>
-      <c r="AG23" s="43"/>
-      <c r="AH23" s="43"/>
-      <c r="AI23" s="43"/>
-      <c r="AJ23" s="43"/>
-      <c r="AK23" s="43"/>
-      <c r="AL23" s="43"/>
+      <c r="B23" s="32" t="s">
+        <v>17</v>
+      </c>
+      <c r="C23" s="32"/>
+      <c r="D23" s="32"/>
+      <c r="E23" s="32"/>
+      <c r="F23" s="32"/>
+      <c r="G23" s="32"/>
+      <c r="H23" s="37"/>
+      <c r="I23" s="37"/>
+      <c r="J23" s="37"/>
+      <c r="K23" s="37"/>
+      <c r="L23" s="37"/>
+      <c r="M23" s="37"/>
+      <c r="N23" s="37"/>
+      <c r="O23" s="37"/>
+      <c r="P23" s="37"/>
+      <c r="Q23" s="37"/>
+      <c r="R23" s="37"/>
+      <c r="S23" s="37"/>
+      <c r="T23" s="37"/>
+      <c r="U23" s="37"/>
+      <c r="V23" s="37"/>
+      <c r="W23" s="37"/>
+      <c r="X23" s="37"/>
+      <c r="Y23" s="37"/>
+      <c r="Z23" s="37"/>
+      <c r="AA23" s="37"/>
+      <c r="AB23" s="37"/>
+      <c r="AC23" s="37"/>
+      <c r="AD23" s="37"/>
+      <c r="AE23" s="37"/>
+      <c r="AF23" s="37"/>
+      <c r="AG23" s="37"/>
+      <c r="AH23" s="37"/>
+      <c r="AI23" s="37"/>
+      <c r="AJ23" s="37"/>
+      <c r="AK23" s="37"/>
+      <c r="AL23" s="37"/>
     </row>
     <row r="24" spans="2:38" ht="11.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="25" spans="2:38" ht="13" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B25" s="40" t="s">
+      <c r="B25" s="34" t="s">
+        <v>18</v>
+      </c>
+      <c r="C25" s="34"/>
+      <c r="D25" s="38" t="s">
         <v>19</v>
       </c>
-      <c r="C25" s="40"/>
-      <c r="D25" s="44" t="s">
+      <c r="E25" s="39"/>
+      <c r="F25" s="39"/>
+      <c r="G25" s="39"/>
+      <c r="H25" s="39"/>
+      <c r="I25" s="39"/>
+      <c r="J25" s="39"/>
+      <c r="K25" s="39"/>
+      <c r="L25" s="39"/>
+      <c r="M25" s="39"/>
+      <c r="N25" s="39"/>
+      <c r="O25" s="39"/>
+      <c r="P25" s="39"/>
+      <c r="Q25" s="39"/>
+      <c r="R25" s="39"/>
+      <c r="S25" s="39"/>
+      <c r="T25" s="39"/>
+      <c r="U25" s="39"/>
+      <c r="V25" s="39"/>
+      <c r="W25" s="39"/>
+      <c r="X25" s="40"/>
+      <c r="Y25" s="35" t="s">
         <v>20</v>
       </c>
-      <c r="E25" s="45"/>
-      <c r="F25" s="45"/>
-      <c r="G25" s="45"/>
-      <c r="H25" s="45"/>
-      <c r="I25" s="45"/>
-      <c r="J25" s="45"/>
-      <c r="K25" s="45"/>
-      <c r="L25" s="45"/>
-      <c r="M25" s="45"/>
-      <c r="N25" s="45"/>
-      <c r="O25" s="45"/>
-      <c r="P25" s="45"/>
-      <c r="Q25" s="45"/>
-      <c r="R25" s="45"/>
-      <c r="S25" s="45"/>
-      <c r="T25" s="45"/>
-      <c r="U25" s="45"/>
-      <c r="V25" s="45"/>
-      <c r="W25" s="45"/>
-      <c r="X25" s="46"/>
-      <c r="Y25" s="41" t="s">
+      <c r="Z25" s="35"/>
+      <c r="AA25" s="35"/>
+      <c r="AB25" s="35" t="s">
         <v>21</v>
       </c>
-      <c r="Z25" s="41"/>
-      <c r="AA25" s="41"/>
-      <c r="AB25" s="41" t="s">
+      <c r="AC25" s="35"/>
+      <c r="AD25" s="35" t="s">
         <v>22</v>
       </c>
-      <c r="AC25" s="41"/>
-      <c r="AD25" s="41" t="s">
+      <c r="AE25" s="35"/>
+      <c r="AF25" s="35"/>
+      <c r="AG25" s="35"/>
+      <c r="AH25" s="36" t="s">
         <v>23</v>
       </c>
-      <c r="AE25" s="41"/>
-      <c r="AF25" s="41"/>
-      <c r="AG25" s="41"/>
-      <c r="AH25" s="42" t="s">
-        <v>24</v>
-      </c>
-      <c r="AI25" s="42"/>
-      <c r="AJ25" s="42"/>
-      <c r="AK25" s="42"/>
-      <c r="AL25" s="42"/>
+      <c r="AI25" s="36"/>
+      <c r="AJ25" s="36"/>
+      <c r="AK25" s="36"/>
+      <c r="AL25" s="36"/>
     </row>
     <row r="26" spans="2:38" s="2" customFormat="1" ht="14" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B26" s="53">
+      <c r="B26" s="24">
         <v>1</v>
       </c>
-      <c r="C26" s="54"/>
-      <c r="D26" s="58"/>
-      <c r="E26" s="59"/>
-      <c r="F26" s="59"/>
-      <c r="G26" s="59"/>
-      <c r="H26" s="59"/>
-      <c r="I26" s="59"/>
-      <c r="J26" s="59"/>
-      <c r="K26" s="59"/>
-      <c r="L26" s="59"/>
-      <c r="M26" s="59"/>
-      <c r="N26" s="59"/>
-      <c r="O26" s="59"/>
-      <c r="P26" s="59"/>
-      <c r="Q26" s="59"/>
-      <c r="R26" s="59"/>
-      <c r="S26" s="59"/>
-      <c r="T26" s="59"/>
-      <c r="U26" s="59"/>
-      <c r="V26" s="59"/>
-      <c r="W26" s="59"/>
-      <c r="X26" s="60"/>
-      <c r="Y26" s="55"/>
-      <c r="Z26" s="56"/>
-      <c r="AA26" s="57"/>
-      <c r="AB26" s="50"/>
-      <c r="AC26" s="51"/>
-      <c r="AD26" s="47"/>
-      <c r="AE26" s="48"/>
-      <c r="AF26" s="48"/>
-      <c r="AG26" s="52"/>
-      <c r="AH26" s="47"/>
-      <c r="AI26" s="48"/>
-      <c r="AJ26" s="48"/>
-      <c r="AK26" s="48"/>
-      <c r="AL26" s="49"/>
+      <c r="C26" s="25"/>
+      <c r="D26" s="29"/>
+      <c r="E26" s="30"/>
+      <c r="F26" s="30"/>
+      <c r="G26" s="30"/>
+      <c r="H26" s="30"/>
+      <c r="I26" s="30"/>
+      <c r="J26" s="30"/>
+      <c r="K26" s="30"/>
+      <c r="L26" s="30"/>
+      <c r="M26" s="30"/>
+      <c r="N26" s="30"/>
+      <c r="O26" s="30"/>
+      <c r="P26" s="30"/>
+      <c r="Q26" s="30"/>
+      <c r="R26" s="30"/>
+      <c r="S26" s="30"/>
+      <c r="T26" s="30"/>
+      <c r="U26" s="30"/>
+      <c r="V26" s="30"/>
+      <c r="W26" s="30"/>
+      <c r="X26" s="31"/>
+      <c r="Y26" s="26"/>
+      <c r="Z26" s="27"/>
+      <c r="AA26" s="28"/>
+      <c r="AB26" s="21"/>
+      <c r="AC26" s="22"/>
+      <c r="AD26" s="18"/>
+      <c r="AE26" s="19"/>
+      <c r="AF26" s="19"/>
+      <c r="AG26" s="23"/>
+      <c r="AH26" s="18"/>
+      <c r="AI26" s="19"/>
+      <c r="AJ26" s="19"/>
+      <c r="AK26" s="19"/>
+      <c r="AL26" s="20"/>
     </row>
     <row r="27" spans="2:38" s="2" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="28" spans="2:38" s="2" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="AG28" s="10" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="AH28" s="13"/>
       <c r="AI28" s="16"/>
@@ -1813,7 +1810,7 @@
     </row>
     <row r="29" spans="2:38" s="2" customFormat="1" ht="14" customHeight="1" x14ac:dyDescent="0.3">
       <c r="AG29" s="10" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="AH29" s="14"/>
       <c r="AI29" s="16"/>
@@ -1854,7 +1851,7 @@
       <c r="AE30" s="6"/>
       <c r="AF30" s="6"/>
       <c r="AG30" s="10" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="AH30" s="14"/>
       <c r="AI30" s="16"/>
@@ -2014,7 +2011,7 @@
     <row r="35" spans="2:38" ht="10" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="36" spans="2:38" s="1" customFormat="1" ht="12.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B36" s="12" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C36" s="12"/>
       <c r="D36" s="12"/>
@@ -2045,7 +2042,7 @@
       <c r="AC36" s="9"/>
       <c r="AD36" s="9"/>
       <c r="AE36" s="9" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="AF36" s="9"/>
       <c r="AG36" s="9"/>
@@ -2066,7 +2063,7 @@
       <c r="I37" s="7"/>
       <c r="J37" s="7"/>
       <c r="K37" s="7" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="L37" s="7"/>
       <c r="M37" s="7"/>
@@ -2079,7 +2076,7 @@
       <c r="T37" s="7"/>
       <c r="U37" s="7"/>
       <c r="V37" s="7" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="W37" s="7"/>
       <c r="X37" s="7"/>
@@ -2090,7 +2087,7 @@
       <c r="AC37" s="11"/>
       <c r="AD37" s="8"/>
       <c r="AE37" s="8" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="AF37" s="11"/>
       <c r="AG37" s="8"/>
@@ -2141,7 +2138,7 @@
     </row>
     <row r="39" spans="2:38" ht="13" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B39" s="12" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C39" s="11"/>
       <c r="D39" s="11"/>
@@ -2172,7 +2169,7 @@
       <c r="AC39" s="9"/>
       <c r="AD39" s="9"/>
       <c r="AE39" s="9" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="AF39" s="9"/>
       <c r="AG39" s="9"/>
@@ -2204,7 +2201,7 @@
       <c r="T40" s="7"/>
       <c r="U40" s="7"/>
       <c r="V40" s="7" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="W40" s="7"/>
       <c r="X40" s="7"/>
@@ -2215,7 +2212,7 @@
       <c r="AC40" s="11"/>
       <c r="AD40" s="8"/>
       <c r="AE40" s="8" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="AF40" s="11"/>
       <c r="AG40" s="8"/>
@@ -2264,91 +2261,83 @@
       <c r="AK41" s="11"/>
       <c r="AL41" s="11"/>
     </row>
-    <row r="42" spans="2:38" ht="13" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B42" s="12" t="s">
-        <v>33</v>
-      </c>
-      <c r="C42" s="12"/>
-      <c r="D42" s="12"/>
-      <c r="E42" s="12"/>
-      <c r="F42" s="12"/>
-      <c r="G42" s="11"/>
-      <c r="H42" s="11"/>
-      <c r="I42" s="11"/>
-      <c r="J42" s="11"/>
-      <c r="K42" s="11"/>
-      <c r="L42" s="11"/>
-      <c r="M42" s="11"/>
-      <c r="N42" s="11"/>
-      <c r="O42" s="11"/>
-      <c r="P42" s="11"/>
-      <c r="Q42" s="11"/>
-      <c r="R42" s="4"/>
-      <c r="S42" s="4"/>
-      <c r="T42" s="4"/>
-      <c r="U42" s="4"/>
-      <c r="V42" s="4"/>
-      <c r="W42" s="4"/>
-      <c r="X42" s="4"/>
-      <c r="Y42" s="4"/>
-      <c r="Z42" s="4"/>
-      <c r="AA42" s="5"/>
-      <c r="AB42" s="11"/>
-      <c r="AC42" s="9"/>
-      <c r="AD42" s="9" t="s">
-        <v>36</v>
-      </c>
-      <c r="AE42" s="9"/>
-      <c r="AF42" s="9"/>
-      <c r="AG42" s="9"/>
-      <c r="AH42" s="9"/>
-      <c r="AI42" s="9"/>
-      <c r="AJ42" s="9"/>
-      <c r="AK42" s="9"/>
-      <c r="AL42" s="9"/>
+    <row r="42" spans="2:38" ht="13" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B42" s="17"/>
+      <c r="C42" s="17"/>
+      <c r="D42" s="17"/>
+      <c r="E42" s="17"/>
+      <c r="F42" s="17"/>
+      <c r="G42" s="17"/>
+      <c r="H42" s="17"/>
+      <c r="I42" s="17"/>
+      <c r="J42" s="17"/>
+      <c r="K42" s="17"/>
+      <c r="L42" s="17"/>
+      <c r="M42" s="17"/>
+      <c r="N42" s="17"/>
+      <c r="O42" s="17"/>
+      <c r="P42" s="17"/>
+      <c r="Q42" s="17"/>
+      <c r="R42" s="17"/>
+      <c r="S42" s="17"/>
+      <c r="T42" s="17"/>
+      <c r="U42" s="17"/>
+      <c r="V42" s="17"/>
+      <c r="W42" s="17"/>
+      <c r="X42" s="17"/>
+      <c r="Y42" s="17"/>
+      <c r="Z42" s="17"/>
+      <c r="AA42" s="17"/>
+      <c r="AB42" s="17"/>
+      <c r="AC42" s="17"/>
+      <c r="AD42" s="17"/>
+      <c r="AE42" s="17"/>
+      <c r="AF42" s="17"/>
+      <c r="AG42" s="17"/>
+      <c r="AH42" s="17"/>
+      <c r="AI42" s="17"/>
+      <c r="AJ42" s="17"/>
+      <c r="AK42" s="17"/>
+      <c r="AL42" s="17"/>
     </row>
     <row r="43" spans="2:38" ht="11" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B43" s="11"/>
-      <c r="C43" s="11"/>
-      <c r="D43" s="11"/>
-      <c r="E43" s="11"/>
-      <c r="F43" s="11"/>
-      <c r="G43" s="11"/>
-      <c r="H43" s="11"/>
-      <c r="I43" s="11"/>
-      <c r="J43" s="11"/>
-      <c r="K43" s="11"/>
-      <c r="L43" s="11"/>
-      <c r="M43" s="11"/>
-      <c r="N43" s="11"/>
-      <c r="O43" s="11"/>
-      <c r="P43" s="11"/>
-      <c r="Q43" s="11"/>
-      <c r="R43" s="11"/>
-      <c r="S43" s="7"/>
-      <c r="T43" s="7"/>
-      <c r="U43" s="7"/>
-      <c r="V43" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="W43" s="7"/>
-      <c r="X43" s="7"/>
-      <c r="Y43" s="7"/>
-      <c r="Z43" s="7"/>
-      <c r="AA43" s="7"/>
-      <c r="AB43" s="11"/>
-      <c r="AC43" s="11"/>
-      <c r="AD43" s="8"/>
-      <c r="AE43" s="8" t="s">
-        <v>31</v>
-      </c>
-      <c r="AF43" s="11"/>
-      <c r="AG43" s="8"/>
-      <c r="AH43" s="8"/>
-      <c r="AI43" s="8"/>
-      <c r="AJ43" s="8"/>
-      <c r="AK43" s="8"/>
-      <c r="AL43" s="8"/>
+      <c r="B43" s="17"/>
+      <c r="C43" s="17"/>
+      <c r="D43" s="17"/>
+      <c r="E43" s="17"/>
+      <c r="F43" s="17"/>
+      <c r="G43" s="17"/>
+      <c r="H43" s="17"/>
+      <c r="I43" s="17"/>
+      <c r="J43" s="17"/>
+      <c r="K43" s="17"/>
+      <c r="L43" s="17"/>
+      <c r="M43" s="17"/>
+      <c r="N43" s="17"/>
+      <c r="O43" s="17"/>
+      <c r="P43" s="17"/>
+      <c r="Q43" s="17"/>
+      <c r="R43" s="17"/>
+      <c r="S43" s="17"/>
+      <c r="T43" s="17"/>
+      <c r="U43" s="17"/>
+      <c r="V43" s="17"/>
+      <c r="W43" s="17"/>
+      <c r="X43" s="17"/>
+      <c r="Y43" s="17"/>
+      <c r="Z43" s="17"/>
+      <c r="AA43" s="17"/>
+      <c r="AB43" s="17"/>
+      <c r="AC43" s="17"/>
+      <c r="AD43" s="17"/>
+      <c r="AE43" s="17"/>
+      <c r="AF43" s="17"/>
+      <c r="AG43" s="17"/>
+      <c r="AH43" s="17"/>
+      <c r="AI43" s="17"/>
+      <c r="AJ43" s="17"/>
+      <c r="AK43" s="17"/>
+      <c r="AL43" s="17"/>
     </row>
     <row r="44" spans="2:38" ht="12" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="45" spans="2:38" ht="13" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2471,7 +2460,7 @@
       <c r="AK50" s="11"/>
       <c r="AL50" s="11"/>
       <c r="AM50" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="51" spans="2:39" ht="9.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -2632,12 +2621,26 @@
     </row>
   </sheetData>
   <mergeCells count="38">
-    <mergeCell ref="AH26:AL26"/>
-    <mergeCell ref="AB26:AC26"/>
-    <mergeCell ref="AD26:AG26"/>
-    <mergeCell ref="B26:C26"/>
-    <mergeCell ref="Y26:AA26"/>
-    <mergeCell ref="D26:X26"/>
+    <mergeCell ref="B1:AL1"/>
+    <mergeCell ref="B3:S4"/>
+    <mergeCell ref="T3:V3"/>
+    <mergeCell ref="W3:AL3"/>
+    <mergeCell ref="T4:V5"/>
+    <mergeCell ref="W4:AL5"/>
+    <mergeCell ref="B5:S5"/>
+    <mergeCell ref="M6:S6"/>
+    <mergeCell ref="T6:V9"/>
+    <mergeCell ref="B15:AL15"/>
+    <mergeCell ref="B17:G17"/>
+    <mergeCell ref="H17:AL17"/>
+    <mergeCell ref="W6:AL9"/>
+    <mergeCell ref="B7:S8"/>
+    <mergeCell ref="B9:S9"/>
+    <mergeCell ref="B11:AL11"/>
+    <mergeCell ref="B13:AL13"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="D6:J6"/>
+    <mergeCell ref="K6:L6"/>
     <mergeCell ref="B19:G19"/>
     <mergeCell ref="H19:AL19"/>
     <mergeCell ref="B21:G21"/>
@@ -2650,26 +2653,12 @@
     <mergeCell ref="AH25:AL25"/>
     <mergeCell ref="H23:AL23"/>
     <mergeCell ref="D25:X25"/>
-    <mergeCell ref="M6:S6"/>
-    <mergeCell ref="T6:V9"/>
-    <mergeCell ref="B15:AL15"/>
-    <mergeCell ref="B17:G17"/>
-    <mergeCell ref="H17:AL17"/>
-    <mergeCell ref="B1:AL1"/>
-    <mergeCell ref="B3:S4"/>
-    <mergeCell ref="T3:V3"/>
-    <mergeCell ref="W3:AL3"/>
-    <mergeCell ref="T4:V5"/>
-    <mergeCell ref="W4:AL5"/>
-    <mergeCell ref="B5:S5"/>
-    <mergeCell ref="W6:AL9"/>
-    <mergeCell ref="B7:S8"/>
-    <mergeCell ref="B9:S9"/>
-    <mergeCell ref="B11:AL11"/>
-    <mergeCell ref="B13:AL13"/>
-    <mergeCell ref="B6:C6"/>
-    <mergeCell ref="D6:J6"/>
-    <mergeCell ref="K6:L6"/>
+    <mergeCell ref="AH26:AL26"/>
+    <mergeCell ref="AB26:AC26"/>
+    <mergeCell ref="AD26:AG26"/>
+    <mergeCell ref="B26:C26"/>
+    <mergeCell ref="Y26:AA26"/>
+    <mergeCell ref="D26:X26"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0" right="0" top="0.19685039370078741" bottom="0" header="0" footer="0"/>

</xml_diff>